<commit_message>
Remove weird FRD+ from KLI source SIT.
</commit_message>
<xml_diff>
--- a/sits/msit_klingon.xlsx
+++ b/sits/msit_klingon.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="981">
   <si>
     <t>Designation</t>
   </si>
@@ -3670,6 +3670,9 @@
   </si>
   <si>
     <t>1-4(6)/None</t>
+  </si>
+  <si>
+    <t>F&amp;E (WTF?)</t>
   </si>
   <si>
     <t>From FRD: 2+6</t>
@@ -4726,8 +4729,8 @@
   </sheetPr>
   <dimension ref="A1:K234"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A69" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A82" activeCellId="0" pane="topLeft" sqref="A82"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A189" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D203" activeCellId="0" pane="topLeft" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11320,7 +11323,7 @@
         <v>855</v>
       </c>
       <c r="D202" s="7" t="s">
-        <v>14</v>
+        <v>856</v>
       </c>
       <c r="E202" s="12" t="n">
         <v>0</v>
@@ -11332,27 +11335,27 @@
         <v>851</v>
       </c>
       <c r="H202" s="7" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="I202" s="7" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="J202" s="13" t="n">
         <v>0</v>
       </c>
       <c r="K202" s="7" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="203">
       <c r="A203" s="4" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B203" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D203" s="4" t="s">
         <v>665</v>
@@ -11370,24 +11373,24 @@
         <v>426</v>
       </c>
       <c r="I203" s="4" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="J203" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K203" s="4" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="204">
       <c r="A204" s="4" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D204" s="4" t="s">
         <v>35</v>
@@ -11402,21 +11405,21 @@
         <v>851</v>
       </c>
       <c r="H204" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="I204" s="4" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="J204" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K204" s="4" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="205">
       <c r="A205" s="3" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
@@ -11431,13 +11434,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="206">
       <c r="A206" s="7" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C206" s="16" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D206" s="7" t="s">
         <v>29</v>
@@ -11449,10 +11452,10 @@
         <v>658</v>
       </c>
       <c r="G206" s="7" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H206" s="7" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="I206" s="7" t="s">
         <v>426</v>
@@ -11461,18 +11464,18 @@
         <v>0</v>
       </c>
       <c r="K206" s="7" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="207">
       <c r="A207" s="7" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B207" s="12" t="n">
         <v>2</v>
       </c>
       <c r="C207" s="16" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="D207" s="7" t="s">
         <v>14</v>
@@ -11484,10 +11487,10 @@
         <v>666</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="H207" s="7" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="I207" s="7" t="s">
         <v>426</v>
@@ -11496,12 +11499,12 @@
         <v>0</v>
       </c>
       <c r="K207" s="7" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="208">
       <c r="A208" s="7" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B208" s="10" t="n">
         <v>24</v>
@@ -11519,7 +11522,7 @@
         <v>850</v>
       </c>
       <c r="G208" s="7" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="H208" s="7" t="s">
         <v>426</v>
@@ -11531,18 +11534,18 @@
         <v>0</v>
       </c>
       <c r="K208" s="7" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="209">
       <c r="A209" s="7" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B209" s="10" t="n">
         <v>24</v>
       </c>
       <c r="C209" s="18" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="D209" s="7" t="s">
         <v>14</v>
@@ -11554,7 +11557,7 @@
         <v>850</v>
       </c>
       <c r="G209" s="7" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="H209" s="7" t="s">
         <v>426</v>
@@ -11566,18 +11569,18 @@
         <v>0</v>
       </c>
       <c r="K209" s="7" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="210">
       <c r="A210" s="7" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B210" s="12" t="n">
         <v>4</v>
       </c>
       <c r="C210" s="16" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="D210" s="7" t="s">
         <v>35</v>
@@ -11595,24 +11598,24 @@
         <v>45</v>
       </c>
       <c r="I210" s="7" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="J210" s="13" t="n">
         <v>0</v>
       </c>
       <c r="K210" s="7" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="211">
       <c r="A211" s="4" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B211" s="5" t="n">
         <v>100</v>
       </c>
       <c r="C211" s="18" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="D211" s="4" t="s">
         <v>29</v>
@@ -11624,10 +11627,10 @@
         <v>472</v>
       </c>
       <c r="G211" s="4" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="H211" s="7" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="I211" s="4" t="s">
         <v>31</v>
@@ -11636,12 +11639,12 @@
         <v>0</v>
       </c>
       <c r="K211" s="4" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="212">
       <c r="A212" s="4" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B212" s="4" t="s">
         <v>69</v>
@@ -11665,24 +11668,24 @@
         <v>426</v>
       </c>
       <c r="I212" s="4" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="J212" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K212" s="4" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="213">
       <c r="A213" s="7" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B213" s="7" t="s">
         <v>408</v>
       </c>
       <c r="C213" s="11" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="D213" s="7" t="s">
         <v>22</v>
@@ -11700,7 +11703,7 @@
         <v>45</v>
       </c>
       <c r="I213" s="7" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="J213" s="13" t="n">
         <v>0</v>
@@ -11711,13 +11714,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="214">
       <c r="A214" s="4" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C214" s="16" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="D214" s="4" t="s">
         <v>113</v>
@@ -11729,30 +11732,30 @@
         <v>36</v>
       </c>
       <c r="G214" s="4" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="H214" s="7" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="I214" s="4" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="J214" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K214" s="4" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="215">
       <c r="A215" s="7" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B215" s="5" t="n">
         <v>17</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D215" s="4" t="s">
         <v>35</v>
@@ -11770,13 +11773,13 @@
         <v>45</v>
       </c>
       <c r="I215" s="4" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="J215" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K215" s="4" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="216">
@@ -11816,13 +11819,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="217">
       <c r="A217" s="7" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B217" s="10" t="n">
         <v>16</v>
       </c>
       <c r="C217" s="11" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="D217" s="7" t="s">
         <v>35</v>
@@ -11840,24 +11843,24 @@
         <v>45</v>
       </c>
       <c r="I217" s="7" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="J217" s="13" t="n">
         <v>0</v>
       </c>
       <c r="K217" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="218">
       <c r="A218" s="4" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C218" s="16" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="D218" s="4" t="s">
         <v>69</v>
@@ -11869,10 +11872,10 @@
         <v>529</v>
       </c>
       <c r="G218" s="4" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="H218" s="7" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="I218" s="4" t="s">
         <v>426</v>
@@ -11881,18 +11884,18 @@
         <v>0</v>
       </c>
       <c r="K218" s="4" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="219">
       <c r="A219" s="4" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C219" s="19" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="D219" s="4" t="s">
         <v>35</v>
@@ -11904,10 +11907,10 @@
         <v>529</v>
       </c>
       <c r="G219" s="4" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="H219" s="7" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="I219" s="4" t="s">
         <v>426</v>
@@ -11916,18 +11919,18 @@
         <v>0</v>
       </c>
       <c r="K219" s="4" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="220">
       <c r="A220" s="4" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B220" s="5" t="n">
         <v>201</v>
       </c>
       <c r="C220" s="18" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="D220" s="4" t="s">
         <v>35</v>
@@ -11939,10 +11942,10 @@
         <v>529</v>
       </c>
       <c r="G220" s="4" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="H220" s="7" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="I220" s="4" t="s">
         <v>426</v>
@@ -11951,18 +11954,18 @@
         <v>0</v>
       </c>
       <c r="K220" s="4" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="221">
       <c r="A221" s="4" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C221" s="16" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="D221" s="4" t="s">
         <v>113</v>
@@ -11974,24 +11977,24 @@
         <v>157</v>
       </c>
       <c r="G221" s="4" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="H221" s="7" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I221" s="4" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="J221" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K221" s="4" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="222">
       <c r="A222" s="3" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
@@ -12006,7 +12009,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="223">
       <c r="A223" s="4" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B223" s="5" t="n">
         <v>14</v>
@@ -12030,24 +12033,24 @@
         <v>426</v>
       </c>
       <c r="I223" s="7" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="J223" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K223" s="4" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="224">
       <c r="A224" s="7" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B224" s="7" t="s">
         <v>408</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="D224" s="7" t="s">
         <v>665</v>
@@ -12062,7 +12065,7 @@
         <v>426</v>
       </c>
       <c r="H224" s="7" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="I224" s="7" t="s">
         <v>408</v>
@@ -12071,12 +12074,12 @@
         <v>0</v>
       </c>
       <c r="K224" s="7" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="225">
       <c r="A225" s="7" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B225" s="7" t="s">
         <v>408</v>
@@ -12100,24 +12103,24 @@
         <v>426</v>
       </c>
       <c r="I225" s="7" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="J225" s="13" t="n">
         <v>0</v>
       </c>
       <c r="K225" s="7" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32" outlineLevel="0" r="226">
       <c r="A226" s="4" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B226" s="5" t="n">
         <v>14</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="D226" s="4" t="s">
         <v>14</v>
@@ -12132,21 +12135,21 @@
         <v>426</v>
       </c>
       <c r="H226" s="4" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="I226" s="7" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="J226" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K226" s="4" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="227">
       <c r="A227" s="3" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B227" s="3"/>
       <c r="C227" s="3"/>
@@ -12161,13 +12164,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="228">
       <c r="A228" s="4" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B228" s="4" t="s">
+        <v>954</v>
+      </c>
+      <c r="C228" s="4" t="s">
         <v>953</v>
-      </c>
-      <c r="C228" s="4" t="s">
-        <v>952</v>
       </c>
       <c r="D228" s="4" t="s">
         <v>29</v>
@@ -12185,24 +12188,24 @@
         <v>426</v>
       </c>
       <c r="I228" s="4" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="J228" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K228" s="4" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="229">
       <c r="A229" s="4" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B229" s="4" t="s">
         <v>408</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="D229" s="4" t="s">
         <v>113</v>
@@ -12220,24 +12223,24 @@
         <v>426</v>
       </c>
       <c r="I229" s="7" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="J229" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K229" s="4" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="230">
       <c r="A230" s="16" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B230" s="7" t="s">
         <v>408</v>
       </c>
       <c r="C230" s="16" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="D230" s="7" t="s">
         <v>35</v>
@@ -12255,24 +12258,24 @@
         <v>426</v>
       </c>
       <c r="I230" s="7" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="J230" s="13" t="n">
         <v>0</v>
       </c>
       <c r="K230" s="7" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="231">
       <c r="A231" s="4" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B231" s="4" t="s">
         <v>408</v>
       </c>
       <c r="C231" s="11" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="D231" s="4" t="s">
         <v>665</v>
@@ -12281,7 +12284,7 @@
         <v>1</v>
       </c>
       <c r="F231" s="7" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="G231" s="4" t="s">
         <v>426</v>
@@ -12290,24 +12293,24 @@
         <v>426</v>
       </c>
       <c r="I231" s="4" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="J231" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K231" s="4" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="232">
       <c r="A232" s="7" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="D232" s="7" t="s">
         <v>665</v>
@@ -12316,7 +12319,7 @@
         <v>0</v>
       </c>
       <c r="F232" s="7" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="G232" s="7" t="s">
         <v>426</v>
@@ -12325,24 +12328,24 @@
         <v>426</v>
       </c>
       <c r="I232" s="7" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="J232" s="13" t="n">
         <v>0</v>
       </c>
       <c r="K232" s="7" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="233">
       <c r="A233" s="7" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="D233" s="7" t="s">
         <v>665</v>
@@ -12351,7 +12354,7 @@
         <v>0</v>
       </c>
       <c r="F233" s="7" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="G233" s="7" t="s">
         <v>426</v>
@@ -12360,18 +12363,18 @@
         <v>426</v>
       </c>
       <c r="I233" s="7" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="J233" s="13" t="n">
         <v>0</v>
       </c>
       <c r="K233" s="7" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="234">
       <c r="A234" s="29" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B234" s="29"/>
       <c r="C234" s="29"/>

</xml_diff>

<commit_message>
Add single-ship carrier note to Klingon B10.
</commit_message>
<xml_diff>
--- a/sits/msit_klingon.xlsx
+++ b/sits/msit_klingon.xlsx
@@ -76,7 +76,7 @@
     <t>Special Rules: 36+8</t>
   </si>
   <si>
-    <t>Base Hull (BB). See (436.0).</t>
+    <t>Base Hull (BB). See (436.0).  Single-Ship Carrier.</t>
   </si>
   <si>
     <t>B10(-)</t>
@@ -4775,8 +4775,8 @@
   </sheetPr>
   <dimension ref="A1:K235"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A200" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H208" activeCellId="0" pane="topLeft" sqref="H208"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L5" activeCellId="0" pane="topLeft" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>